<commit_message>
without xcel working code
</commit_message>
<xml_diff>
--- a/EdisonLogs/src/testdatalogin.xlsx
+++ b/EdisonLogs/src/testdatalogin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="6915"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="11175"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -40,28 +40,10 @@
     <t>tyu1223</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
     <t>pass</t>
-  </si>
-  <si>
-    <t>text 2</t>
-  </si>
-  <si>
-    <t>text 3</t>
-  </si>
-  <si>
-    <t>text 4</t>
-  </si>
-  <si>
-    <t>text 5</t>
   </si>
 </sst>
 </file>
@@ -98,7 +80,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -409,19 +401,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="6" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.59375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="6.44140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="6.44140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="8" max="9" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="6.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,82 +426,82 @@
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
       <c r="F1" s="5"/>
-      <c r="G1" t="s" s="6">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s" s="7">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s" s="8">
-        <v>9</v>
+      <c r="G1" s="6"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="8"/>
+      <c r="J1" t="s" s="9">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s" s="10">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="M1" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s" s="13">
+        <v>7</v>
+      </c>
+      <c r="O1" t="s" s="14">
+        <v>7</v>
+      </c>
+      <c r="P1" t="s" s="15">
+        <v>7</v>
+      </c>
+      <c r="Q1" t="s" s="16">
+        <v>7</v>
+      </c>
+      <c r="R1" t="s" s="17">
+        <v>7</v>
+      </c>
+      <c r="S1" t="s" s="18">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
         <v>8</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>